<commit_message>
fix: HASSUYP-351: Korjaa migraatio
</commit_message>
<xml_diff>
--- a/migration-cli/migraatioTemplate.xlsx
+++ b/migration-cli/migraatioTemplate.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\phakala\hassu\migration-cli\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F490FAB-DAFF-49F2-BFF1-E7C923A105AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="7155" yWindow="4125" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Migraatio" sheetId="1" r:id="rId4"/>
+    <sheet name="Migraatio" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>oid</t>
   </si>
@@ -31,34 +40,23 @@
     <t>1. Jatkopäätös päivämäärä</t>
   </si>
   <si>
-    <t>1.2.246.578.5.1.2512564980.479402805</t>
+    <t>1.2.246.578.5.1.2978288874.2711575506</t>
   </si>
   <si>
-    <t>SUUNNITTELU</t>
+    <t>NAHTAVILLAOLO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="d.m.yyyy"/>
-    <numFmt numFmtId="60" formatCode="d.m.yyyy h.mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="d\.m\.yyyy"/>
+    <numFmt numFmtId="165" formatCode="d\.m\.yyyy\ h\.mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -107,29 +105,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -138,24 +122,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -357,7 +402,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -375,7 +420,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -404,7 +449,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -429,7 +474,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -454,7 +499,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -479,7 +524,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -504,7 +549,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -529,7 +574,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -554,7 +599,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -579,7 +624,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -604,7 +649,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -617,9 +662,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -636,7 +687,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -654,7 +705,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -679,7 +730,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -704,7 +755,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -729,7 +780,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -754,7 +805,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -779,7 +830,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -804,7 +855,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -829,7 +880,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -854,7 +905,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -879,7 +930,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -892,9 +943,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -908,7 +965,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -926,7 +983,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,7 +1012,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -980,7 +1037,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +1062,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1030,7 +1087,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1055,7 +1112,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1080,7 +1137,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1105,7 +1162,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1130,7 +1187,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1155,7 +1212,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1168,58 +1225,68 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="40.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.8516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.3516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="15.4" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="22" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:6" ht="21.95" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2"/>
@@ -1227,7 +1294,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" ht="15.35" customHeight="1">
+    <row r="3" spans="1:6" ht="15.4" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1235,7 +1302,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" ht="15.35" customHeight="1">
+    <row r="4" spans="1:6" ht="15.4" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1243,7 +1310,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" ht="15.35" customHeight="1">
+    <row r="5" spans="1:6" ht="15.4" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1251,7 +1318,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" ht="15.35" customHeight="1">
+    <row r="6" spans="1:6" ht="15.4" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1259,7 +1326,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" ht="15.35" customHeight="1">
+    <row r="7" spans="1:6" ht="15.4" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1267,7 +1334,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" ht="15.35" customHeight="1">
+    <row r="8" spans="1:6" ht="15.4" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1275,7 +1342,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" ht="15.35" customHeight="1">
+    <row r="9" spans="1:6" ht="15.4" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1283,7 +1350,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" ht="15.35" customHeight="1">
+    <row r="10" spans="1:6" ht="15.4" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1293,14 +1360,20 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"SUUNNITTELU,Tila"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
fix: HASSUYP-351: Korjaa migraatio (#1252)
</commit_message>
<xml_diff>
--- a/migration-cli/migraatioTemplate.xlsx
+++ b/migration-cli/migraatioTemplate.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\phakala\hassu\migration-cli\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F490FAB-DAFF-49F2-BFF1-E7C923A105AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="7155" yWindow="4125" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Migraatio" sheetId="1" r:id="rId4"/>
+    <sheet name="Migraatio" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>oid</t>
   </si>
@@ -31,34 +40,23 @@
     <t>1. Jatkopäätös päivämäärä</t>
   </si>
   <si>
-    <t>1.2.246.578.5.1.2512564980.479402805</t>
+    <t>1.2.246.578.5.1.2978288874.2711575506</t>
   </si>
   <si>
-    <t>SUUNNITTELU</t>
+    <t>NAHTAVILLAOLO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="d.m.yyyy"/>
-    <numFmt numFmtId="60" formatCode="d.m.yyyy h.mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="d\.m\.yyyy"/>
+    <numFmt numFmtId="165" formatCode="d\.m\.yyyy\ h\.mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -107,29 +105,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -138,24 +122,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -357,7 +402,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -375,7 +420,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -404,7 +449,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -429,7 +474,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -454,7 +499,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -479,7 +524,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -504,7 +549,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -529,7 +574,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -554,7 +599,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -579,7 +624,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -604,7 +649,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -617,9 +662,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -636,7 +687,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -654,7 +705,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -679,7 +730,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -704,7 +755,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -729,7 +780,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -754,7 +805,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -779,7 +830,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -804,7 +855,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -829,7 +880,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -854,7 +905,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -879,7 +930,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -892,9 +943,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -908,7 +965,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -926,7 +983,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,7 +1012,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -980,7 +1037,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +1062,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1030,7 +1087,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1055,7 +1112,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1080,7 +1137,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1105,7 +1162,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1130,7 +1187,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1155,7 +1212,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1168,58 +1225,68 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="40.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.8516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.3516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="15.4" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="22" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:6" ht="21.95" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2"/>
@@ -1227,7 +1294,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" ht="15.35" customHeight="1">
+    <row r="3" spans="1:6" ht="15.4" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1235,7 +1302,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" ht="15.35" customHeight="1">
+    <row r="4" spans="1:6" ht="15.4" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1243,7 +1310,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" ht="15.35" customHeight="1">
+    <row r="5" spans="1:6" ht="15.4" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1251,7 +1318,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" ht="15.35" customHeight="1">
+    <row r="6" spans="1:6" ht="15.4" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1259,7 +1326,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" ht="15.35" customHeight="1">
+    <row r="7" spans="1:6" ht="15.4" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1267,7 +1334,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" ht="15.35" customHeight="1">
+    <row r="8" spans="1:6" ht="15.4" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1275,7 +1342,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" ht="15.35" customHeight="1">
+    <row r="9" spans="1:6" ht="15.4" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1283,7 +1350,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" ht="15.35" customHeight="1">
+    <row r="10" spans="1:6" ht="15.4" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1293,14 +1360,20 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"SUUNNITTELU,Tila"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
päivitä exceliin data validointia
</commit_message>
<xml_diff>
--- a/migration-cli/migraatioTemplate.xlsx
+++ b/migration-cli/migraatioTemplate.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomi/Projects/hassu/migration-cli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C432C17-20E7-F046-A86B-5127F836E6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7BD981-1879-D04A-B121-F9C0E02DC163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4120" windowWidth="34560" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="34560" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Migraatio" sheetId="1" r:id="rId1"/>
+    <sheet name="Migraatiot" sheetId="1" r:id="rId1"/>
     <sheet name="Tilat" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>oid</t>
   </si>
@@ -41,9 +41,6 @@
     <t>1. Jatkopäätös päivämäärä</t>
   </si>
   <si>
-    <t>1.2.246.578.5.1.2978288874.2711575506</t>
-  </si>
-  <si>
     <t>NAHTAVILLAOLO</t>
   </si>
   <si>
@@ -58,25 +55,28 @@
   <si>
     <t>JATKOPAATOS2</t>
   </si>
+  <si>
+    <t>TESTI-ASIA-123</t>
+  </si>
+  <si>
+    <t>1.2.246.578.5.1.2293640800.1682339657</t>
+  </si>
+  <si>
+    <t>TESTI-ASIA-243</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="d\.m\.yyyy"/>
-    <numFmt numFmtId="165" formatCode="d\.m\.yyyy\ h\.mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="12"/>
@@ -85,21 +85,15 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -107,145 +101,183 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="10"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="10"/>
+        </left>
+        <right style="thin">
+          <color indexed="10"/>
+        </right>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="10"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="10"/>
+        </left>
+        <right style="thin">
+          <color indexed="10"/>
+        </right>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="10"/>
+        </left>
+        <right style="thin">
+          <color indexed="10"/>
+        </right>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="10"/>
+        </right>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -264,211 +296,10 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="10"/>
-        </left>
-        <right style="thin">
-          <color indexed="10"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="d\.m\.yyyy\ h\.mm"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="10"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="10"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="10"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="10"/>
-        </left>
-        <right style="thin">
-          <color indexed="10"/>
-        </right>
-        <top style="thin">
-          <color indexed="10"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="10"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="d\.m\.yyyy\ h\.mm"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="10"/>
-        </left>
-        <right style="thin">
-          <color indexed="10"/>
-        </right>
-        <top style="thin">
-          <color indexed="10"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="10"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="10"/>
-        </left>
-        <right style="thin">
-          <color indexed="10"/>
-        </right>
-        <top style="thin">
-          <color indexed="10"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="10"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="10"/>
-        </left>
-        <right style="thin">
-          <color indexed="10"/>
-        </right>
-        <top style="thin">
-          <color indexed="10"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="10"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="10"/>
-        </right>
-        <top style="thin">
-          <color indexed="10"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="10"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="10"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="10"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="10"/>
-        </left>
-        <right style="thin">
-          <color indexed="10"/>
-        </right>
-        <top style="thin">
-          <color indexed="10"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="10"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
-  <tableStyles count="0"/>
+  <tableStyles count="1" defaultTableStyle="Table Style 1">
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{F86B91CE-BE50-F64B-AE89-0C999E04F53D}"/>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -548,23 +379,27 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ABB9076D-BEE3-6B45-AD05-4691416E5F82}" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:F10" xr:uid="{ABB9076D-BEE3-6B45-AD05-4691416E5F82}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ABB9076D-BEE3-6B45-AD05-4691416E5F82}" name="Migraatiot" displayName="Migraatiot" ref="A1:F13" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:F13" xr:uid="{ABB9076D-BEE3-6B45-AD05-4691416E5F82}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{65A74F41-0582-3C4A-BE50-893116F8E7CB}" name="oid" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{740AF809-B31E-6943-BEA4-59B943F5E91D}" name="Tila" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{F73D5B16-BF03-2A47-8879-9F453ED830E4}" name="Hyväksymispäätös asianumero" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{2A599E33-2CEB-E34A-8736-9579FCD9774D}" name="Hyväksymispäätös päivämäärä" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{95479D72-6DDA-A445-8EFA-6D472F375C5B}" name="1. Jatkopäätös asianumero" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{A2E04996-0D35-A74D-956E-A982720F384F}" name="1. Jatkopäätös päivämäärä" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{65A74F41-0582-3C4A-BE50-893116F8E7CB}" name="oid" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{740AF809-B31E-6943-BEA4-59B943F5E91D}" name="Tila" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{F73D5B16-BF03-2A47-8879-9F453ED830E4}" name="Hyväksymispäätös asianumero" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{2A599E33-2CEB-E34A-8736-9579FCD9774D}" name="Hyväksymispäätös päivämäärä" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{95479D72-6DDA-A445-8EFA-6D472F375C5B}" name="1. Jatkopäätös asianumero" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{A2E04996-0D35-A74D-956E-A982720F384F}" name="1. Jatkopäätös päivämäärä" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{75E9B83B-6632-B74B-BF6F-BBF9263111F4}" name="Table2" displayName="Table2" ref="A1:A6" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{75E9B83B-6632-B74B-BF6F-BBF9263111F4}" name="Tilat" displayName="Tilat" ref="A1:A6" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:A6" xr:uid="{75E9B83B-6632-B74B-BF6F-BBF9263111F4}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{9847349E-D6BF-174C-8995-F3DC7AA4A4D6}" name="Tila"/>
@@ -1618,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1635,103 +1470,98 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>6</v>
+    <row r="2" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44611</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5">
+        <v>44606</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="5"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="5"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="5"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="5"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="17"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B13" xr:uid="{EFE67CDC-6FC0-3545-862B-9EC4A4058E34}">
+      <formula1>INDIRECT("Tilat[Tila]")</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
@@ -1748,7 +1578,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A2:A6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1757,33 +1587,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HASSUYP-721 Migraatiotyökaluun tuki 2. jatkopäätökseen meneville projekteille (#1487)
* wip

* päivitä exceliin data validointia

---------

Co-authored-by: tomi korkalainen <tomi.korkalainen@cgi.com>
</commit_message>
<xml_diff>
--- a/migration-cli/migraatioTemplate.xlsx
+++ b/migration-cli/migraatioTemplate.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\phakala\hassu\migration-cli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomi/Projects/hassu/migration-cli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F490FAB-DAFF-49F2-BFF1-E7C923A105AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7BD981-1879-D04A-B121-F9C0E02DC163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7155" yWindow="4125" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="34560" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Migraatio" sheetId="1" r:id="rId1"/>
+    <sheet name="Migraatiot" sheetId="1" r:id="rId1"/>
+    <sheet name="Tilat" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>oid</t>
   </si>
@@ -40,67 +41,64 @@
     <t>1. Jatkopäätös päivämäärä</t>
   </si>
   <si>
-    <t>1.2.246.578.5.1.2978288874.2711575506</t>
+    <t>NAHTAVILLAOLO</t>
   </si>
   <si>
-    <t>NAHTAVILLAOLO</t>
+    <t>SUUNNITTELU</t>
+  </si>
+  <si>
+    <t>HYVAKSYMISPAATOS</t>
+  </si>
+  <si>
+    <t>JATKOPAATOS1</t>
+  </si>
+  <si>
+    <t>JATKOPAATOS2</t>
+  </si>
+  <si>
+    <t>TESTI-ASIA-123</t>
+  </si>
+  <si>
+    <t>1.2.246.578.5.1.2293640800.1682339657</t>
+  </si>
+  <si>
+    <t>TESTI-ASIA-243</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="d\.m\.yyyy"/>
-    <numFmt numFmtId="165" formatCode="d\.m\.yyyy\ h\.mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -110,16 +108,198 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="10"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="10"/>
+        </left>
+        <right style="thin">
+          <color indexed="10"/>
+        </right>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="10"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="10"/>
+        </left>
+        <right style="thin">
+          <color indexed="10"/>
+        </right>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="10"/>
+        </left>
+        <right style="thin">
+          <color indexed="10"/>
+        </right>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="10"/>
+        </right>
+        <top style="thin">
+          <color indexed="10"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="10"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="Table Style 1">
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{F86B91CE-BE50-F64B-AE89-0C999E04F53D}"/>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -197,6 +377,35 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ABB9076D-BEE3-6B45-AD05-4691416E5F82}" name="Migraatiot" displayName="Migraatiot" ref="A1:F13" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:F13" xr:uid="{ABB9076D-BEE3-6B45-AD05-4691416E5F82}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{65A74F41-0582-3C4A-BE50-893116F8E7CB}" name="oid" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{740AF809-B31E-6943-BEA4-59B943F5E91D}" name="Tila" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{F73D5B16-BF03-2A47-8879-9F453ED830E4}" name="Hyväksymispäätös asianumero" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{2A599E33-2CEB-E34A-8736-9579FCD9774D}" name="Hyväksymispäätös päivämäärä" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{95479D72-6DDA-A445-8EFA-6D472F375C5B}" name="1. Jatkopäätös asianumero" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{A2E04996-0D35-A74D-956E-A982720F384F}" name="1. Jatkopäätös päivämäärä" dataDxfId="0" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{75E9B83B-6632-B74B-BF6F-BBF9263111F4}" name="Tilat" displayName="Tilat" ref="A1:A6" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A1:A6" xr:uid="{75E9B83B-6632-B74B-BF6F-BBF9263111F4}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{9847349E-D6BF-174C-8995-F3DC7AA4A4D6}" name="Tila"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1244,124 +1453,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="4" max="4" width="28.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="25.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.4" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="21.95" customHeight="1">
+    <row r="2" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.4" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44611</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5">
+        <v>44606</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="5"/>
-      <c r="E3" s="2"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="15.4" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+    <row r="4" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="5"/>
-      <c r="E4" s="2"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.4" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+    <row r="5" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="5"/>
-      <c r="E5" s="2"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15.4" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+    <row r="6" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="5"/>
-      <c r="E6" s="2"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="15.4" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+    <row r="7" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="15.4" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+    <row r="8" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="15.4" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+    <row r="9" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="15.4" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+    <row r="10" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="5"/>
-      <c r="E10" s="2"/>
       <c r="F10" s="5"/>
     </row>
+    <row r="11" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
   </sheetData>
+  <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"SUUNNITTELU,Tila"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B13" xr:uid="{EFE67CDC-6FC0-3545-862B-9EC4A4058E34}">
+      <formula1>INDIRECT("Tilat[Tila]")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1369,6 +1567,60 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70402203-528D-AB40-AB89-78F1BA770611}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>